<commit_message>
Modification at 2024-05-14 22:26:37
</commit_message>
<xml_diff>
--- a/Variables.xlsx
+++ b/Variables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16640"/>
+    <workbookView windowHeight="17120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
   <si>
     <t>Field</t>
   </si>
@@ -52,7 +52,7 @@
     <t>Msun/yr</t>
   </si>
   <si>
-    <t>Star formation rate of this age. Note that the non-zero star formation rate at the last age has no time to take any effect.</t>
+    <t>Star formation rate of this age. Note that the non-zero star formation rate at the last age has no time to take any effect. The star formation is assumed to be instantaneous.</t>
   </si>
   <si>
     <t>TimeBin</t>
@@ -64,13 +64,13 @@
     <t>Mstar</t>
   </si>
   <si>
-    <t>The total mass of the newly formed stars during the epoch from this age to the next age, which is SFR*TimeBin. Note that it will always be zeors for the last age as TimeBin is set to be zero for the last age.</t>
+    <t>The total mass of the newly formed stars during the epoch just after this age, which is SFR*TimeBin. Note that it will always be zeors for the last age as TimeBin is set to be zero for the last age.</t>
   </si>
   <si>
     <t>Nstar</t>
   </si>
   <si>
-    <t>The number of of the newly formed stars during the epoch from this age to the next age. Note that it will always be zeros for the last age as TimeBin is set to be zero for the last age.</t>
+    <t>The number of of the newly formed stars during the epoch just after this age. Note that it will always be zeros for the last age as TimeBin is set to be zero for the last age.</t>
   </si>
   <si>
     <t>YieldsTable</t>
@@ -109,7 +109,25 @@
     <t>EjectElement</t>
   </si>
   <si>
-    <t>The mass of H, He, Li, ..., Zn, and other metals of the ejecta at each ages. Here the `ejecta` also includes the winds from AGB stars.  It includes the ejecta from all already formed stars.  The index of element starts from 1. For instance, GasElement[0,1] is the mass of H in the first age. GasElement[:,0] is set to be zero.</t>
+    <t>The mass of H, He, Li, ..., Zn, and other metals of the ejecta from this age to the next age. Here the `ejecta` also includes the winds from AGB stars.  It includes the ejecta from all already formed stars. For instance, EjectElement[5,1] is the total mass of ejecta of H up to the 6th age. The index of element starts from 1 and GasElement[:,0] is set to be zero.</t>
+  </si>
+  <si>
+    <t>dEjectElement</t>
+  </si>
+  <si>
+    <t>dEjectElement[i,:] indicates the ejecta during Age[i] and Age[i+1] of the stellar population formed just after Age[j]. This variable won't be output. It will be initilized to be zero before calculation the ejceta of each epoch. If j&lt;i, dEjectElement is zero.</t>
+  </si>
+  <si>
+    <t>SNIaNum</t>
+  </si>
+  <si>
+    <t>The total number of SNIa events from this age to the next age</t>
+  </si>
+  <si>
+    <t>dSNIaNum</t>
+  </si>
+  <si>
+    <t>Similar to dEjectElement, but for the number of the SNIa events.</t>
   </si>
   <si>
     <t>ZGas</t>
@@ -121,19 +139,16 @@
     <t>IMF</t>
   </si>
   <si>
+    <t>numpy arrray or str</t>
+  </si>
+  <si>
     <t>Msun, 1</t>
   </si>
   <si>
-    <t>(N, 2)</t>
-  </si>
-  <si>
-    <t>The first column is the initial mass, while the second is the IMF</t>
-  </si>
-  <si>
-    <t>SNIaNum</t>
-  </si>
-  <si>
-    <t>The number of SNIa events from this age to the next age</t>
+    <t>(N, 2), 1</t>
+  </si>
+  <si>
+    <t>The first column is the initial mass, while the second is the IMF. If it is a string, it should be either of 'Salpeter', 'Chabrier', 'Kroupa', 'PowerLaw' (with power index provided) or 'DietSalpeter'.</t>
   </si>
 </sst>
 </file>
@@ -1281,10 +1296,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -1329,7 +1344,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" ht="34" spans="1:5">
+    <row r="3" ht="51" spans="1:5">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1448,7 +1463,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" ht="68" spans="1:5">
+    <row r="10" ht="84" spans="1:5">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1465,18 +1480,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" ht="17" spans="1:5">
+    <row r="11" ht="51" spans="1:5">
       <c r="A11" t="s">
         <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>33</v>
@@ -1489,19 +1504,19 @@
       <c r="B12" t="s">
         <v>24</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="D12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" ht="17" spans="1:5">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
         <v>24</v>
@@ -1513,7 +1528,41 @@
         <v>8</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" ht="17" spans="1:5">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="15" ht="51" spans="1:5">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modification at 2024-05-21 22:33:35
</commit_message>
<xml_diff>
--- a/Variables.xlsx
+++ b/Variables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17120"/>
+    <workbookView windowWidth="28000" windowHeight="16640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="47">
   <si>
     <t>Field</t>
   </si>
@@ -145,10 +145,16 @@
     <t>Msun, 1</t>
   </si>
   <si>
-    <t>(N, 2), 1</t>
+    <t>(N, 2) or 1</t>
   </si>
   <si>
     <t>The first column is the initial mass, while the second is the IMF. If it is a string, it should be either of 'Salpeter', 'Chabrier', 'Kroupa', 'PowerLaw' (with power index provided) or 'DietSalpeter'.</t>
+  </si>
+  <si>
+    <t>StellarMass</t>
+  </si>
+  <si>
+    <t>StellarMass[i] is the stellar mass just after Age[i]</t>
   </si>
 </sst>
 </file>
@@ -1296,10 +1302,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -1565,6 +1571,23 @@
         <v>44</v>
       </c>
     </row>
+    <row r="16" ht="17" spans="1:5">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>